<commit_message>
PREGUNTA 7, EN LOS DATOS actualizados tengo nueva data para uso.
</commit_message>
<xml_diff>
--- a/data/Incendios-Forestales-2021.xlsx
+++ b/data/Incendios-Forestales-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP 15\Downloads\Samsung\Repositorio\sic-forest-fire-rd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THE FSR\source\repos\sic-forest-fire-rd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CB1C0-A76E-48C1-B439-F97499C536D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA05683-9953-40EB-A088-59401EAEF7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9C335E22-CF0A-E849-BFB8-AAA567361A93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9C335E22-CF0A-E849-BFB8-AAA567361A93}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="247">
   <si>
     <t>no.</t>
   </si>
@@ -771,6 +769,15 @@
   </si>
   <si>
     <t>No Intencional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Gastos por m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -823,7 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -840,9 +847,15 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -859,9 +872,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -899,7 +912,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1005,7 +1018,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1147,7 +1160,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1155,31 +1168,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87353C5-2ABF-6842-BB28-922F55B6FC01}">
-  <dimension ref="A1:N251"/>
+  <dimension ref="A1:P251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D194" workbookViewId="0">
-      <selection activeCell="G202" sqref="G202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="10.85546875" style="3"/>
+    <col min="3" max="3" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="10.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1222,8 +1235,12 @@
       <c r="N1" s="3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1268,8 +1285,9 @@
         <f xml:space="preserve"> TEXT(L2, "mmm-yyyy")</f>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1314,8 +1332,11 @@
         <f t="shared" ref="N3:N66" si="1" xml:space="preserve"> TEXT(L3, "mmm-yyyy")</f>
         <v>01/13/2021</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1360,8 +1381,11 @@
         <f t="shared" si="1"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1406,8 +1430,11 @@
         <f t="shared" si="1"/>
         <v>01/16/2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1452,8 +1479,11 @@
         <f t="shared" si="1"/>
         <v>01/15/2021</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1498,8 +1528,11 @@
         <f t="shared" si="1"/>
         <v>01/17/2021</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1544,8 +1577,11 @@
         <f t="shared" si="1"/>
         <v>01/18/2021</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1590,8 +1626,11 @@
         <f t="shared" si="1"/>
         <v>01/23/2021</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1636,8 +1675,11 @@
         <f t="shared" si="1"/>
         <v>01/25/2021</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1682,8 +1724,11 @@
         <f t="shared" si="1"/>
         <v>01/25/2021</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1728,8 +1773,11 @@
         <f t="shared" si="1"/>
         <v>01/27/2021</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1774,8 +1822,11 @@
         <f t="shared" si="1"/>
         <v>01/27/2021</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1820,8 +1871,11 @@
         <f t="shared" si="1"/>
         <v>01/26/2021</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1866,8 +1920,11 @@
         <f t="shared" si="1"/>
         <v>01/26/2021</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1912,8 +1969,11 @@
         <f t="shared" si="1"/>
         <v>01/20/2021</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1958,8 +2018,11 @@
         <f t="shared" si="1"/>
         <v>01/20/2021</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2004,8 +2067,11 @@
         <f t="shared" si="1"/>
         <v>01/24/2021</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2050,8 +2116,11 @@
         <f t="shared" si="1"/>
         <v>01/24/2021</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2096,8 +2165,11 @@
         <f t="shared" si="1"/>
         <v>01/24/2021</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2142,8 +2214,11 @@
         <f t="shared" si="1"/>
         <v>01/18/2021</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2188,8 +2263,11 @@
         <f t="shared" si="1"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2234,8 +2312,11 @@
         <f t="shared" si="1"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2280,8 +2361,11 @@
         <f t="shared" si="1"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2326,8 +2410,11 @@
         <f t="shared" si="1"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2372,8 +2459,11 @@
         <f t="shared" si="1"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2418,8 +2508,11 @@
         <f t="shared" si="1"/>
         <v>02/16/2021</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2464,8 +2557,11 @@
         <f t="shared" si="1"/>
         <v>02/15/2021</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2510,8 +2606,11 @@
         <f t="shared" si="1"/>
         <v>02/19/2021</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2556,8 +2655,11 @@
         <f t="shared" si="1"/>
         <v>02/20/2021</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2602,8 +2704,11 @@
         <f t="shared" si="1"/>
         <v>02/22/2021</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2648,8 +2753,11 @@
         <f t="shared" si="1"/>
         <v>02/23/2021</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2694,8 +2802,11 @@
         <f t="shared" si="1"/>
         <v>02/22/2021</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2740,8 +2851,11 @@
         <f t="shared" si="1"/>
         <v>02/17/2021</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2786,8 +2900,11 @@
         <f t="shared" si="1"/>
         <v>02/19/2021</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2832,8 +2949,11 @@
         <f t="shared" si="1"/>
         <v>02/24/2021</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2878,8 +2998,11 @@
         <f t="shared" si="1"/>
         <v>02/21/2021</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2924,8 +3047,11 @@
         <f t="shared" si="1"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2970,8 +3096,11 @@
         <f t="shared" si="1"/>
         <v>02/25/2021</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3016,8 +3145,11 @@
         <f t="shared" si="1"/>
         <v>02/19/2021</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3062,8 +3194,11 @@
         <f t="shared" si="1"/>
         <v>02/25/2021</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3108,8 +3243,11 @@
         <f t="shared" si="1"/>
         <v>02/28/2021</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3154,8 +3292,11 @@
         <f t="shared" si="1"/>
         <v>02/20/2021</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3200,8 +3341,11 @@
         <f t="shared" si="1"/>
         <v>02/21/2021</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3246,8 +3390,11 @@
         <f t="shared" si="1"/>
         <v>02/19/2021</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3292,8 +3439,11 @@
         <f t="shared" si="1"/>
         <v>02/26/2021</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3338,8 +3488,11 @@
         <f t="shared" si="1"/>
         <v>02/28/2021</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3384,8 +3537,11 @@
         <f t="shared" si="1"/>
         <v>02/26/2021</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3430,8 +3586,11 @@
         <f t="shared" si="1"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3476,8 +3635,11 @@
         <f t="shared" si="1"/>
         <v>02/26/2021</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3522,8 +3684,11 @@
         <f t="shared" si="1"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3568,8 +3733,11 @@
         <f t="shared" si="1"/>
         <v>dic-2021</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3614,8 +3782,11 @@
         <f t="shared" si="1"/>
         <v>02/27/2021</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3660,8 +3831,11 @@
         <f t="shared" si="1"/>
         <v>02/20/2021</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3706,8 +3880,11 @@
         <f t="shared" si="1"/>
         <v>02/26/2021</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3752,8 +3929,11 @@
         <f t="shared" si="1"/>
         <v>02/27/2021</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3798,8 +3978,11 @@
         <f t="shared" si="1"/>
         <v>02/26/2021</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3844,8 +4027,11 @@
         <f t="shared" si="1"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3890,8 +4076,11 @@
         <f t="shared" si="1"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3936,8 +4125,11 @@
         <f t="shared" si="1"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3982,8 +4174,11 @@
         <f t="shared" si="1"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4028,8 +4223,11 @@
         <f t="shared" si="1"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4074,8 +4272,11 @@
         <f t="shared" si="1"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4120,8 +4321,11 @@
         <f t="shared" si="1"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4166,8 +4370,11 @@
         <f t="shared" si="1"/>
         <v>02/28/2021</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4212,8 +4419,11 @@
         <f t="shared" si="1"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4258,8 +4468,11 @@
         <f t="shared" ref="N67:N130" si="3" xml:space="preserve"> TEXT(L67, "mmm-yyyy")</f>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4304,8 +4517,11 @@
         <f t="shared" si="3"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4350,8 +4566,11 @@
         <f t="shared" si="3"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4396,8 +4615,11 @@
         <f t="shared" si="3"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4442,8 +4664,11 @@
         <f t="shared" si="3"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4488,8 +4713,11 @@
         <f t="shared" si="3"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4534,8 +4762,11 @@
         <f t="shared" si="3"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4580,8 +4811,11 @@
         <f t="shared" si="3"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4626,8 +4860,11 @@
         <f t="shared" si="3"/>
         <v>oct-2021</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4672,8 +4909,11 @@
         <f t="shared" si="3"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4718,8 +4958,11 @@
         <f t="shared" si="3"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4764,8 +5007,11 @@
         <f t="shared" si="3"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4810,8 +5056,11 @@
         <f t="shared" si="3"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4856,8 +5105,11 @@
         <f t="shared" si="3"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4902,8 +5154,11 @@
         <f t="shared" si="3"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4948,8 +5203,11 @@
         <f t="shared" si="3"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4994,8 +5252,11 @@
         <f t="shared" si="3"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5040,8 +5301,11 @@
         <f t="shared" si="3"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5086,8 +5350,11 @@
         <f t="shared" si="3"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5132,8 +5399,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5178,8 +5448,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5224,8 +5497,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5270,8 +5546,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5316,8 +5595,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5362,8 +5644,11 @@
         <f t="shared" si="3"/>
         <v>03/16/2021</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5408,8 +5693,11 @@
         <f t="shared" si="3"/>
         <v>03/20/2021</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5454,8 +5742,11 @@
         <f t="shared" si="3"/>
         <v>03/21/2021</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5500,8 +5791,11 @@
         <f t="shared" si="3"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5546,8 +5840,11 @@
         <f t="shared" si="3"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5592,8 +5889,11 @@
         <f t="shared" si="3"/>
         <v>03/19/2021</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5638,8 +5938,11 @@
         <f t="shared" si="3"/>
         <v>03/20/2021</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5684,8 +5987,11 @@
         <f t="shared" si="3"/>
         <v>03/19/2021</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5730,8 +6036,11 @@
         <f t="shared" si="3"/>
         <v>03/21/2021</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -5776,8 +6085,11 @@
         <f t="shared" si="3"/>
         <v>03/15/2021</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5822,8 +6134,11 @@
         <f t="shared" si="3"/>
         <v>03/26/2021</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -5868,8 +6183,11 @@
         <f t="shared" si="3"/>
         <v>03/26/2021</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5914,8 +6232,11 @@
         <f t="shared" si="3"/>
         <v>03/29/2021</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5960,8 +6281,11 @@
         <f t="shared" si="3"/>
         <v>03/28/2021</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -6006,8 +6330,11 @@
         <f t="shared" si="3"/>
         <v>03/29/2021</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -6052,8 +6379,11 @@
         <f t="shared" si="3"/>
         <v>03/28/2021</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -6098,8 +6428,11 @@
         <f t="shared" si="3"/>
         <v>03/26/2021</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -6144,8 +6477,11 @@
         <f t="shared" si="3"/>
         <v>03/31/2021</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -6190,8 +6526,11 @@
         <f t="shared" si="3"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -6236,8 +6575,11 @@
         <f t="shared" si="3"/>
         <v>03/30/2021</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -6282,8 +6624,11 @@
         <f t="shared" si="3"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O111" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -6328,8 +6673,11 @@
         <f t="shared" si="3"/>
         <v>04/18/2021</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6374,8 +6722,11 @@
         <f t="shared" si="3"/>
         <v>04/18/2021</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6420,8 +6771,11 @@
         <f t="shared" si="3"/>
         <v>04/18/2021</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6466,8 +6820,11 @@
         <f t="shared" si="3"/>
         <v>04/15/2021</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6512,8 +6869,11 @@
         <f t="shared" si="3"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -6558,8 +6918,11 @@
         <f t="shared" si="3"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -6604,8 +6967,11 @@
         <f t="shared" si="3"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -6650,8 +7016,11 @@
         <f t="shared" si="3"/>
         <v>04/21/2021</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -6696,8 +7065,11 @@
         <f t="shared" si="3"/>
         <v>04/21/2021</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -6742,8 +7114,11 @@
         <f t="shared" si="3"/>
         <v>04/22/2021</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -6788,8 +7163,11 @@
         <f t="shared" si="3"/>
         <v>04/20/2021</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -6834,8 +7212,11 @@
         <f t="shared" si="3"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -6880,8 +7261,11 @@
         <f t="shared" si="3"/>
         <v>04/13/2021</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -6926,8 +7310,11 @@
         <f t="shared" si="3"/>
         <v>04/18/2021</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -6972,8 +7359,11 @@
         <f t="shared" si="3"/>
         <v>04/15/2021</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O126" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -7018,8 +7408,11 @@
         <f t="shared" si="3"/>
         <v>04/15/2021</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O127" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -7064,8 +7457,11 @@
         <f t="shared" si="3"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O128" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -7110,8 +7506,11 @@
         <f t="shared" si="3"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O129" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -7156,8 +7555,11 @@
         <f t="shared" si="3"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O130" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -7202,8 +7604,11 @@
         <f t="shared" ref="N131:N194" si="5" xml:space="preserve"> TEXT(L131, "mmm-yyyy")</f>
         <v>04/23/2021</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O131" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -7248,8 +7653,11 @@
         <f t="shared" si="5"/>
         <v>04/21/2021</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O132" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -7294,8 +7702,11 @@
         <f t="shared" si="5"/>
         <v>04/19/2021</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O133" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -7340,8 +7751,11 @@
         <f t="shared" si="5"/>
         <v>04/17/2021</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O134" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -7386,8 +7800,11 @@
         <f t="shared" si="5"/>
         <v>nov-2021</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O135" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -7432,8 +7849,11 @@
         <f t="shared" si="5"/>
         <v>04/19/2021</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O136" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -7478,8 +7898,11 @@
         <f t="shared" si="5"/>
         <v>04/21/2021</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O137" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -7524,8 +7947,11 @@
         <f t="shared" si="5"/>
         <v>oct-2021</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O138" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -7570,8 +7996,11 @@
         <f t="shared" si="5"/>
         <v>04/13/2021</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O139" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -7616,8 +8045,11 @@
         <f t="shared" si="5"/>
         <v>04/24/2021</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O140" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -7662,8 +8094,11 @@
         <f t="shared" si="5"/>
         <v>04/25/2021</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O141" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -7708,8 +8143,11 @@
         <f t="shared" si="5"/>
         <v>04/26/2021</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O142" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -7754,8 +8192,11 @@
         <f t="shared" si="5"/>
         <v>dic-2021</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O143" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -7800,8 +8241,11 @@
         <f t="shared" si="5"/>
         <v>04/20/2021</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O144" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -7846,8 +8290,11 @@
         <f t="shared" si="5"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O145" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -7892,8 +8339,11 @@
         <f t="shared" si="5"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O146" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -7938,8 +8388,11 @@
         <f t="shared" si="5"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O147" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -7984,8 +8437,11 @@
         <f t="shared" si="5"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O148" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -8030,8 +8486,11 @@
         <f t="shared" si="5"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O149" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -8076,8 +8535,11 @@
         <f t="shared" si="5"/>
         <v>oct-2021</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O150" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -8122,8 +8584,11 @@
         <f t="shared" si="5"/>
         <v>oct-2021</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O151" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -8168,8 +8633,11 @@
         <f t="shared" si="5"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O152" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -8214,8 +8682,11 @@
         <f t="shared" si="5"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O153" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -8260,8 +8731,11 @@
         <f t="shared" si="5"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O154" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -8306,8 +8780,11 @@
         <f t="shared" si="5"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O155" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -8352,8 +8829,11 @@
         <f t="shared" si="5"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O156" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -8398,8 +8878,11 @@
         <f t="shared" si="5"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O157" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -8444,8 +8927,11 @@
         <f t="shared" si="5"/>
         <v>feb-2021</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O158" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -8490,8 +8976,11 @@
         <f t="shared" si="5"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O159" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -8536,8 +9025,11 @@
         <f t="shared" si="5"/>
         <v>05/16/2021</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O160" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -8582,8 +9074,11 @@
         <f t="shared" si="5"/>
         <v>05/16/2021</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O161" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -8628,8 +9123,11 @@
         <f t="shared" si="5"/>
         <v>05/15/2021</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O162" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -8674,8 +9172,11 @@
         <f t="shared" si="5"/>
         <v>05/14/2021</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O163" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -8720,8 +9221,11 @@
         <f t="shared" si="5"/>
         <v>05/15/2021</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O164" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -8766,8 +9270,11 @@
         <f t="shared" si="5"/>
         <v>05/14/2021</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O165" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -8812,8 +9319,11 @@
         <f t="shared" si="5"/>
         <v>05/14/2021</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O166" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -8858,8 +9368,11 @@
         <f t="shared" si="5"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O167" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -8904,8 +9417,11 @@
         <f t="shared" si="5"/>
         <v>05/15/2021</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O168" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -8950,8 +9466,11 @@
         <f t="shared" si="5"/>
         <v>05/18/2021</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O169" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -8996,8 +9515,11 @@
         <f t="shared" si="5"/>
         <v>05/17/2021</v>
       </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O170" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -9042,8 +9564,11 @@
         <f t="shared" si="5"/>
         <v>05/17/2021</v>
       </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O171" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -9088,8 +9613,11 @@
         <f t="shared" si="5"/>
         <v>05/24/2021</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O172" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -9134,8 +9662,11 @@
         <f t="shared" si="5"/>
         <v>06/19/2021</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O173" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -9180,8 +9711,11 @@
         <f t="shared" si="5"/>
         <v>06/28/2021</v>
       </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O174" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -9226,8 +9760,11 @@
         <f t="shared" si="5"/>
         <v>06/29/2021</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O175" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -9272,8 +9809,11 @@
         <f t="shared" si="5"/>
         <v>06/25/2021</v>
       </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O176" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -9318,8 +9858,11 @@
         <f t="shared" si="5"/>
         <v>06/25/2021</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O177" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -9364,8 +9907,11 @@
         <f t="shared" si="5"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O178" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -9410,8 +9956,11 @@
         <f t="shared" si="5"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O179" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -9456,8 +10005,11 @@
         <f t="shared" si="5"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O180" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -9502,8 +10054,11 @@
         <f t="shared" si="5"/>
         <v>07/13/2021</v>
       </c>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O181" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -9548,8 +10103,11 @@
         <f t="shared" si="5"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O182" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -9594,8 +10152,11 @@
         <f t="shared" si="5"/>
         <v>07/17/2021</v>
       </c>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O183" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -9640,8 +10201,11 @@
         <f t="shared" si="5"/>
         <v>07/13/2021</v>
       </c>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O184" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -9686,8 +10250,11 @@
         <f t="shared" si="5"/>
         <v>07/21/2021</v>
       </c>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O185" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -9732,8 +10299,11 @@
         <f t="shared" si="5"/>
         <v>07/26/2021</v>
       </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O186" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -9778,8 +10348,11 @@
         <f t="shared" si="5"/>
         <v>07/31/2021</v>
       </c>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O187" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -9824,8 +10397,11 @@
         <f t="shared" si="5"/>
         <v>mar-2021</v>
       </c>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O188" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -9870,8 +10446,11 @@
         <f t="shared" si="5"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O189" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -9916,8 +10495,11 @@
         <f t="shared" si="5"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O190" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -9962,8 +10544,11 @@
         <f t="shared" si="5"/>
         <v>08/14/2021</v>
       </c>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O191" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -10008,8 +10593,11 @@
         <f t="shared" si="5"/>
         <v>08/14/2021</v>
       </c>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O192" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -10054,8 +10642,11 @@
         <f t="shared" si="5"/>
         <v>08/14/2021</v>
       </c>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O193" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -10100,8 +10691,11 @@
         <f t="shared" si="5"/>
         <v>08/14/2021</v>
       </c>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O194" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -10146,8 +10740,11 @@
         <f t="shared" ref="N195:N251" si="7" xml:space="preserve"> TEXT(L195, "mmm-yyyy")</f>
         <v>08/15/2021</v>
       </c>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O195" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -10192,8 +10789,11 @@
         <f t="shared" si="7"/>
         <v>08/21/2021</v>
       </c>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O196" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -10238,8 +10838,11 @@
         <f t="shared" si="7"/>
         <v>08/22/2021</v>
       </c>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O197" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -10284,8 +10887,11 @@
         <f t="shared" si="7"/>
         <v>08/25/2021</v>
       </c>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O198" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -10330,8 +10936,11 @@
         <f t="shared" si="7"/>
         <v>08/24/2021</v>
       </c>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O199" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -10376,8 +10985,11 @@
         <f t="shared" si="7"/>
         <v>08/18/2021</v>
       </c>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O200" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -10422,8 +11034,11 @@
         <f t="shared" si="7"/>
         <v>08/27/2021</v>
       </c>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O201" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -10468,8 +11083,11 @@
         <f t="shared" si="7"/>
         <v>08/27/2021</v>
       </c>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O202" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -10514,8 +11132,11 @@
         <f t="shared" si="7"/>
         <v>oct-2021</v>
       </c>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O203" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -10560,8 +11181,11 @@
         <f t="shared" si="7"/>
         <v>08/14/2021</v>
       </c>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O204" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -10606,8 +11230,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O205" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -10652,8 +11279,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O206" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -10698,8 +11328,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O207" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -10744,8 +11377,11 @@
         <f t="shared" si="7"/>
         <v>08/28/2021</v>
       </c>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O208" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -10790,8 +11426,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O209" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -10836,8 +11475,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O210" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -10882,8 +11524,11 @@
         <f t="shared" si="7"/>
         <v>08/30/2021</v>
       </c>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O211" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -10928,8 +11573,11 @@
         <f t="shared" si="7"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O212" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -10974,8 +11622,11 @@
         <f t="shared" si="7"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O213" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -11020,8 +11671,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O214" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -11066,8 +11720,11 @@
         <f t="shared" si="7"/>
         <v>08/31/2021</v>
       </c>
-    </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O215" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -11112,8 +11769,11 @@
         <f t="shared" si="7"/>
         <v>08/31/2021</v>
       </c>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O216" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -11158,8 +11818,11 @@
         <f t="shared" si="7"/>
         <v>08/29/2021</v>
       </c>
-    </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O217" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -11204,8 +11867,11 @@
         <f t="shared" si="7"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O218" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -11250,8 +11916,11 @@
         <f t="shared" si="7"/>
         <v>jul-2021</v>
       </c>
-    </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O219" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -11296,8 +11965,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O220" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -11342,8 +12014,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O221" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -11388,8 +12063,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O222" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -11434,8 +12112,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O223" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -11480,8 +12161,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O224" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -11526,8 +12210,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O225" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -11572,8 +12259,11 @@
         <f t="shared" si="7"/>
         <v>ago-2021</v>
       </c>
-    </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O226" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -11618,8 +12308,11 @@
         <f t="shared" si="7"/>
         <v>jun-2021</v>
       </c>
-    </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O227" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -11664,8 +12357,11 @@
         <f t="shared" si="7"/>
         <v>09/15/2021</v>
       </c>
-    </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O228" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -11710,8 +12406,11 @@
         <f t="shared" si="7"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O229" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -11756,8 +12455,11 @@
         <f t="shared" si="7"/>
         <v>10/25/2021</v>
       </c>
-    </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O230" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -11802,8 +12504,11 @@
         <f t="shared" si="7"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O231" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -11848,8 +12553,11 @@
         <f t="shared" si="7"/>
         <v>may-2021</v>
       </c>
-    </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O232" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -11894,8 +12602,11 @@
         <f t="shared" si="7"/>
         <v>abr-2021</v>
       </c>
-    </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O233" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -11940,8 +12651,11 @@
         <f t="shared" si="7"/>
         <v>sep-2021</v>
       </c>
-    </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O234" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -11986,8 +12700,11 @@
         <f t="shared" si="7"/>
         <v>11/19/2021</v>
       </c>
-    </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O235" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -12032,8 +12749,11 @@
         <f t="shared" si="7"/>
         <v>11/20/2021</v>
       </c>
-    </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O236" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -12078,8 +12798,11 @@
         <f t="shared" si="7"/>
         <v>11/22/2021</v>
       </c>
-    </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O237" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -12124,8 +12847,11 @@
         <f t="shared" si="7"/>
         <v>11/26/2021</v>
       </c>
-    </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O238" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -12170,8 +12896,11 @@
         <f t="shared" si="7"/>
         <v>11/24/2021</v>
       </c>
-    </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O239" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -12216,8 +12945,11 @@
         <f t="shared" si="7"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O240" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -12262,8 +12994,11 @@
         <f t="shared" si="7"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O241" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -12308,8 +13043,11 @@
         <f t="shared" si="7"/>
         <v>11/13/2021</v>
       </c>
-    </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O242" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -12354,8 +13092,11 @@
         <f t="shared" si="7"/>
         <v>ene-2021</v>
       </c>
-    </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O243" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -12400,8 +13141,11 @@
         <f t="shared" si="7"/>
         <v>12/14/2021</v>
       </c>
-    </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O244" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -12446,8 +13190,11 @@
         <f t="shared" si="7"/>
         <v>dic-2021</v>
       </c>
-    </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O245" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -12492,8 +13239,11 @@
         <f t="shared" si="7"/>
         <v>12/20/2021</v>
       </c>
-    </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O246" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -12538,8 +13288,11 @@
         <f t="shared" si="7"/>
         <v>12/19/2021</v>
       </c>
-    </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O247" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -12584,8 +13337,11 @@
         <f t="shared" si="7"/>
         <v>12/17/2021</v>
       </c>
-    </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O248" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -12630,8 +13386,11 @@
         <f t="shared" si="7"/>
         <v>12/18/2021</v>
       </c>
-    </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O249" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -12676,8 +13435,11 @@
         <f t="shared" si="7"/>
         <v>12/20/2021</v>
       </c>
-    </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O250" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -12722,9 +13484,15 @@
         <f t="shared" si="7"/>
         <v>12/21/2021</v>
       </c>
+      <c r="O251" s="6" t="s">
+        <v>246</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N251" xr:uid="{A87353C5-2ABF-6842-BB28-922F55B6FC01}"/>
+  <mergeCells count="1">
+    <mergeCell ref="O1:P1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>